<commit_message>
watchservice og noget andet
</commit_message>
<xml_diff>
--- a/src/files/MOCK_DATA1.xlsx
+++ b/src/files/MOCK_DATA1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\IdeaProjects\ArlaFoodsEsbjergExam\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\ArlaFoodsEsbjergExam\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21559894-75BA-4E0A-B747-92E0A302FEAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EF70D2-BB95-47A5-BD2B-8F1DD334CC15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="696" yWindow="156" windowWidth="13344" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Monday</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Sunday</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Amount in Liters</t>
   </si>
 </sst>
 </file>
@@ -390,67 +396,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
       </c>
       <c r="B3">
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>750</v>
       </c>
     </row>

</xml_diff>